<commit_message>
working on changing string
</commit_message>
<xml_diff>
--- a/Anand_Work/FallWork2018/Provider_survey_data.xlsx
+++ b/Anand_Work/FallWork2018/Provider_survey_data.xlsx
@@ -23145,8 +23145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CEL48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H35" zoomScale="67" workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="67" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>